<commit_message>
com.twilio.video.VideoView cannot be cast to android.widget.VideoView
</commit_message>
<xml_diff>
--- a/Staj Dosyalarım/Copy of Staj Boş Format_x (4).xlsx
+++ b/Staj Dosyalarım/Copy of Staj Boş Format_x (4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baris\Desktop\staj\Staj Dosyalarım\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F586EB-9146-46CA-A467-0117659D69F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E21143-7BD3-49BA-803A-4ED2D2A6FA55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,7 +605,7 @@
         <v>30</v>
       </c>
       <c r="Q2" s="3">
-        <v>44044</v>
+        <v>44075</v>
       </c>
       <c r="R2" s="1">
         <v>44057</v>

</xml_diff>